<commit_message>
start readme and upload screenshot
</commit_message>
<xml_diff>
--- a/Tables.xlsx
+++ b/Tables.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dw00830/Desktop/sei/projects/AndyProject2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FD29439-B4A5-2A4E-83B5-D63BF50DBA0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2518A76D-9CF3-6941-9264-E0DD67F3788A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3300" yWindow="500" windowWidth="28040" windowHeight="18880" activeTab="1" xr2:uid="{631C2DC0-EFEE-EB45-B81C-C505F4F2CF98}"/>
+    <workbookView xWindow="3280" yWindow="500" windowWidth="28040" windowHeight="18680" activeTab="1" xr2:uid="{631C2DC0-EFEE-EB45-B81C-C505F4F2CF98}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2 (2)" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="66">
   <si>
     <t>USERS</t>
   </si>
@@ -55,9 +56,6 @@
     <t>name</t>
   </si>
   <si>
-    <t>userName</t>
-  </si>
-  <si>
     <t>password</t>
   </si>
   <si>
@@ -91,18 +89,12 @@
     <t>GIVERS</t>
   </si>
   <si>
-    <t>giverId</t>
-  </si>
-  <si>
     <t>address</t>
   </si>
   <si>
     <t>gifts</t>
   </si>
   <si>
-    <t>noteSent</t>
-  </si>
-  <si>
     <t>BOOLEAN</t>
   </si>
   <si>
@@ -211,9 +203,6 @@
     <t>ADD GIVER</t>
   </si>
   <si>
-    <t>/newgiver</t>
-  </si>
-  <si>
     <t>Gift</t>
   </si>
   <si>
@@ -223,13 +212,28 @@
     <t>EDIT GIVER</t>
   </si>
   <si>
-    <t>/editgiver</t>
-  </si>
-  <si>
     <t>GIVER INDEX</t>
   </si>
   <si>
-    <t>/giverindex</t>
+    <t>givername</t>
+  </si>
+  <si>
+    <t>giverid</t>
+  </si>
+  <si>
+    <t>notesent</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>/newgiver.ejs</t>
+  </si>
+  <si>
+    <t>/giverindex.ejs</t>
+  </si>
+  <si>
+    <t>/editgiver.ejs</t>
   </si>
 </sst>
 </file>
@@ -1316,6 +1320,1169 @@
     </mc:AlternateContent>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>273400</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>37700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>663340</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>41360</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId29">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="39" name="Ink 38">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA7572C0-A862-5D45-A77C-091AAC3C4E7F}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="8757000" y="8051400"/>
+            <a:ext cx="3171240" cy="1641960"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="39" name="Ink 38">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA7572C0-A862-5D45-A77C-091AAC3C4E7F}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId30"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="8721360" y="8015760"/>
+              <a:ext cx="3242880" cy="1713600"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>418560</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>20800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>555280</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>150780</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId31">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="41" name="Ink 40">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{24BD9564-F9B1-4849-A8DB-566C00785743}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="7200360" y="5151600"/>
+            <a:ext cx="1838520" cy="1361880"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="41" name="Ink 40">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{24BD9564-F9B1-4849-A8DB-566C00785743}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId32"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7164720" y="5115960"/>
+              <a:ext cx="1910160" cy="1433520"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>241720</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>42900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>139160</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>144860</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId33">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="44" name="Ink 43">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{18C00BEF-54CE-3641-9DBE-7E1B04627C6A}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="10554120" y="5796000"/>
+            <a:ext cx="1675440" cy="914760"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="44" name="Ink 43">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{18C00BEF-54CE-3641-9DBE-7E1B04627C6A}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId34"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="10518480" y="5760360"/>
+              <a:ext cx="1747080" cy="986400"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>555640</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>135800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>331300</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>53940</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId35">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="45" name="Ink 44">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9280C938-1E46-F040-BE52-140EC6D890C4}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="14297040" y="5063400"/>
+            <a:ext cx="2252160" cy="1353240"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="45" name="Ink 44">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9280C938-1E46-F040-BE52-140EC6D890C4}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId36"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="14261040" y="5027760"/>
+              <a:ext cx="2323800" cy="1424880"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>511740</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>163420</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>124800</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>40500</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId37">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="48" name="Ink 47">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EB133FEF-38FA-7544-8F43-00039CE69BD4}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="4740840" y="6932520"/>
+            <a:ext cx="2165760" cy="2137680"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="48" name="Ink 47">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EB133FEF-38FA-7544-8F43-00039CE69BD4}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId38"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="4704840" y="6896520"/>
+              <a:ext cx="2237400" cy="2209320"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>312460</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>47280</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>170860</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>154260</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId39">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="50" name="Ink 49">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B3772529-A05E-2248-B74D-E45B18D1DF45}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="1137960" y="7438680"/>
+            <a:ext cx="1611000" cy="1745280"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="50" name="Ink 49">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B3772529-A05E-2248-B74D-E45B18D1DF45}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId40"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="1101960" y="7403040"/>
+              <a:ext cx="1682640" cy="1816920"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>721020</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>104940</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>127420</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>19680</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="2" name="Ink 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F99A1774-A803-9B41-A416-779DCE407530}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="3197520" y="1133640"/>
+            <a:ext cx="2784600" cy="1553040"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="2" name="Ink 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F99A1774-A803-9B41-A416-779DCE407530}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3188520" y="1125000"/>
+              <a:ext cx="2802240" cy="1570680"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Graphic 2" descr="Checkbox Checked with solid fill">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{45C985AD-CEF9-444C-94B8-812C3110909D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId4"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4229100" y="8191500"/>
+          <a:ext cx="266700" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>425380</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>108060</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>386480</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>190520</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="4" name="Ink 3">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F3F916C1-B414-9D4D-B3B2-745401278B9A}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="3003480" y="3803760"/>
+            <a:ext cx="786600" cy="1314360"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="4" name="Ink 3">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F3F916C1-B414-9D4D-B3B2-745401278B9A}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2994840" y="3795120"/>
+              <a:ext cx="804240" cy="1332000"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>301160</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>98700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>611820</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>25800</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="5" name="Ink 4">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D9C074D-0212-8D40-A832-DEA2F65B1A08}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="3704760" y="3794400"/>
+            <a:ext cx="1136160" cy="955800"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="5" name="Ink 4">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D9C074D-0212-8D40-A832-DEA2F65B1A08}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3696120" y="3785400"/>
+              <a:ext cx="1153800" cy="973440"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>767740</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>40900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>2760</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>32100</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="6" name="Ink 5">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{882C0292-98B7-534E-B4A0-C33917F2CFAB}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="3345840" y="5590800"/>
+            <a:ext cx="3438720" cy="194400"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="6" name="Ink 5">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{882C0292-98B7-534E-B4A0-C33917F2CFAB}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3336840" y="5581800"/>
+              <a:ext cx="3456360" cy="212040"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>306560</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>561400</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>181200</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId11">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="7" name="Ink 6">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{23ADD0D0-A66B-F644-B8C4-166B7C819788}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="3710160" y="6769800"/>
+            <a:ext cx="5334840" cy="802800"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="7" name="Ink 6">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{23ADD0D0-A66B-F644-B8C4-166B7C819788}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3701160" y="6761160"/>
+              <a:ext cx="5352480" cy="820440"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>437600</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>97140</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>628360</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>42080</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId13">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="8" name="Ink 7">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8F6736C0-80E2-7846-BF77-BFD9CD8B46B1}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="3841200" y="6459840"/>
+            <a:ext cx="1841760" cy="1176840"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="8" name="Ink 7">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8F6736C0-80E2-7846-BF77-BFD9CD8B46B1}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3832200" y="6451200"/>
+              <a:ext cx="1859400" cy="1194480"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>428600</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>48140</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>556720</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId15">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="9" name="Ink 8">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FFD95F76-D1B7-AD41-8A35-ED8306FFA9E3}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="12519000" y="6004440"/>
+            <a:ext cx="1779120" cy="167760"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="9" name="Ink 8">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FFD95F76-D1B7-AD41-8A35-ED8306FFA9E3}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="12510000" y="5995440"/>
+              <a:ext cx="1796760" cy="185400"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>761020</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>120500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>35140</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>46400</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId17">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="10" name="Ink 9">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BB77F2F7-40B5-3442-87C2-E91E9AC98D8C}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="1586520" y="6076800"/>
+            <a:ext cx="1026720" cy="1564200"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="10" name="Ink 9">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BB77F2F7-40B5-3442-87C2-E91E9AC98D8C}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="1577880" y="6067800"/>
+              <a:ext cx="1044360" cy="1581840"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>322900</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>104900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>27940</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>190120</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId19">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="11" name="Ink 10">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3067BDED-F8B8-104B-A604-F22072B94755}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="1148400" y="727200"/>
+            <a:ext cx="1457640" cy="1926720"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="11" name="Ink 10">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3067BDED-F8B8-104B-A604-F22072B94755}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="1139400" y="718560"/>
+              <a:ext cx="1475280" cy="1944360"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>614680</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>25060</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>611440</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>176980</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId21">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="12" name="Ink 11">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{38B9FE00-9808-024D-BB76-B87FFF5165D3}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="9098280" y="5574960"/>
+            <a:ext cx="1825560" cy="151920"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="12" name="Ink 11">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{38B9FE00-9808-024D-BB76-B87FFF5165D3}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId22"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="9089640" y="5565960"/>
+              <a:ext cx="1843200" cy="169560"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>458140</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>86020</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>430720</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>200580</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId23">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="13" name="Ink 12">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BB840D3C-2F08-3248-B559-298BE65C80B5}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="3036240" y="911520"/>
+            <a:ext cx="2449080" cy="927360"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="13" name="Ink 12">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BB840D3C-2F08-3248-B559-298BE65C80B5}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId24"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3000600" y="875880"/>
+              <a:ext cx="2520720" cy="999000"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1460,6 +2627,174 @@
 </inkml:ink>
 </file>
 
+<file path=xl/ink/ink14.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2021-08-22T01:08:52.096"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.2" units="cm"/>
+      <inkml:brushProperty name="height" value="0.2" units="cm"/>
+      <inkml:brushProperty name="color" value="#008C3A"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 2358 24575,'4'30'0,"31"35"0,5-18 0,5 13 0,-18-8 0,1 3 0,1-12 0,3 4-383,-1 15 1,1 7 0,1-6 382,5-11 0,1 3 0,8 27 0,3 15 0,-7-12 0,-16-29 0,0 2-656,6 7 1,9 16-1,3 6 1,-1-3 0,-6-11-438,0-5 1,-4-7 0,1 3 674,10 21 0,2 4 0,-3-8 1309,4-3 0,-5-13-891,-1-5 0,3 4 0,-12-44 389,-28-30-389,32-30 0,29-26 0,11-6 0,-9 13 0,7 7 0,7-2 345,-24 12 1,9-8 0,7-7-1,4-2 1,1 0 0,-1 3 0,-5 6-346,15-5 0,-2 5 0,0 2 0,1 1 0,-1-2-547,-12 7 1,1-1 0,0 1 0,-1-1 0,1 0 0,0-1 202,0 0 0,-1-1 1,1-1-1,0 1 1,1 0-1,0 0 344,2 0 0,-1 3 0,1-1 0,2-1 0,5-3 0,8-4-274,-21 9 1,7-3 0,4-2 0,3-3 0,3-1 0,2-1 0,0-1 0,0 0 0,-2 2 0,-1 0 0,-4 3 0,-4 2 240,4-2 1,-3 2-1,-2 2 1,-3 0-1,0 2 1,1-2-1,1 0 1,2-3-1,4-2-166,-5 2 0,5-3 0,3-2 0,2-3 0,2 0 0,-1 0 0,-1 0 0,-2 2 1,-3 2-1,-6 2 0,-5 4 0,-7 5 199,16-11 0,-9 7 0,-7 3 0,-1 1 0,2-2 31,19-12 0,1-1 1,-4 2-1,-7 6-31,-14 8 0,-6 4 0,3 2 816,10-1 1,3 1-1,7-5-816,1-4 0,11-8 0,3-2 0,-6 3 0,-14 9 0,7-1 0,-2 1 409,0-2 1,19-11-1,1-2 1,-19 10-1,-40 20 1,-36 20 0,-4 1-1</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink15.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2021-08-22T02:15:18.169"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.2" units="cm"/>
+      <inkml:brushProperty name="height" value="0.2" units="cm"/>
+      <inkml:brushProperty name="color" value="#008C3A"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 3247 24575,'0'35'0,"0"18"0,5-1 0,14 20 0,-5-34 0,22 16 0,-10-16 0,19 8 0,-13-10 0,9 0 0,-6-18 0,1 10 0,10-21 0,3 3 0,9-4 0,24-5 0,6 5-1213,-9-14 1,6-10 1212,-5-12 0,2-9-1093,-2-2 1,6-8 0,-2-5 812,-21 8 0,-3-4 0,1-3 0,1-2-540,11-7 1,2-3 0,0-2 0,0-2 590,-12 8 1,0-2-1,1-1 1,-1 0-1,2-1-383,4-2 0,0-1 0,2 0 0,-1 0 0,0-2 612,-9 8 0,0 0 0,-1-1 0,1-1 0,0 1 0,-1 1-249,0 2 1,0-1-1,-1 1 1,1 1-1,0 0 1,-1 0 248,12-10 0,0-1 0,0 2 0,-2 2 0,-3 2-24,2 1 0,-4 3 0,0 1 0,1 0 24,6-5 0,2 0 0,-1 2 0,-3 3 350,4-2 0,-2 5 0,-2 1-350,-5 4 0,-1 2 0,-1-1 589,0-2 1,-1 1 0,-4 4-590,5 1 0,-4 3 1466,3-7 1,-2-1-1467,-5 9 0,-3 3 3276,11-10-2938,-12 12 2500,-23 20-2838,-6 6 580,-19 23 1,0-8 0,-10 12-1</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink16.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2021-08-22T02:15:34.090"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.2" units="cm"/>
+      <inkml:brushProperty name="height" value="0.2" units="cm"/>
+      <inkml:brushProperty name="color" value="#008C3A"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">6 1423 24575,'-5'35'0,"10"19"0,3 5 0,19 23 0,9 3-1237,7 1 1237,-17-34 0,1 1 0,-5-4 0,1-1 0,6 3 0,2-1 0,-1-4 0,0-2 0,21 20 0,-11-17 0,3-4 0,22 5 0,-21-11 0,3-4 0,3-15 0,4-7 0,22-2 0,6-4-1214,3 0 0,5-3 1214,-14-1 0,4-2 0,0-8-1093,8-13 1,1-8 0,2-5 889,-16 7 0,2-2 0,1-4 0,1-3-453,-6-2 1,1-4-1,1-4 1,1 0 0,-1-2 467,6-3 0,1-2 1,0-1-1,0-2 0,1-1-237,-10 4 1,2-1 0,0-1-1,-1-1 1,-2 1 0,-3 2 424,0 1 0,-3 1 0,-1 1 0,-1-1 0,1-4-155,9-10 1,2-7-1,-1 1 1,-5 3-1,-8 9 155,-6 7 0,-7 7 0,2-5 132,5-8 1,3-7 0,0 1 0,-6 8-133,7-4 0,-4 4 1087,10-17 1,-2 2-1088,-19 22 0,-4 6 3276,13-14-2641,-16 16 2641,-17 30-2593,-7 3 2452,-5 9-3135,0 0 0,-4 0 0,-1 0 0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink17.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2021-08-23T18:49:09.710"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.2" units="cm"/>
+      <inkml:brushProperty name="height" value="0.2" units="cm"/>
+      <inkml:brushProperty name="color" value="#008C3A"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">0 3245 24575,'45'29'0,"14"8"0,22 21-1369,-37-25 1,2 0 1368,12 0 0,2 0 0,-5 2 0,3-1 0,15-3 0,4-2-866,-1 1 1,2-2 865,4-8 0,3-4 0,8-1 0,6-4-842,-11-6 1,5-3-1,-1-1 842,-8 0 0,0-1 0,4-1 0,-7 1 0,4-1 0,1-1 0,-2-5-820,-5-4 1,-1-5 0,-1-2 0,3-3 722,7-2 0,1-4 1,1-2-1,-1-6-456,-13 1 0,0-4 0,0-3 0,0-2 0,1-1 553,7-5 0,1-2 0,0-3 0,0-1 0,-1-2-296,-14 6 0,-1-1 1,-1-2-1,0-1 1,1-1-1,0-1 296,5-4 0,0-2 0,0 0 0,1-2 0,-2 0 0,-1-2-138,1-2 1,-1-3 0,-1-1 0,-1 1 0,-2 1 0,-3 2 137,0 1 0,-4 2 0,-2 1 0,0 0 0,1-3 0,6-7 0,1-3 0,0-1 0,-4 2 0,-4 4 95,-8 5 0,-4 3 0,-3 2 1,1 0-96,15-17 0,-2 1 0,0 0 445,0-1 1,-2 0 0,-6 7-446,-7 5 0,-3 4 1255,14-9 1,-1 3-1256,-19 18 0,-3 5 3276,18-15-2247,-24 20 2247,-9 21-3107,-5 7 2655,-1 9-2824,0 1 1216,-4 8-1216,-1 11 0,-4 14 0,0-9 0,0 1 0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink18.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2021-08-24T02:37:33.661"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.2" units="cm"/>
+      <inkml:brushProperty name="height" value="0.2" units="cm"/>
+      <inkml:brushProperty name="color" value="#008C3A"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">0 4966 24575,'0'29'0,"11"7"0,2 5 0,18 15 0,-5-6 0,11 13 0,-16-15 0,-3-1 0,5 8 0,6-1 0,-1 0 0,-8-6 0,11-2 0,4 1 0,7 11 0,11 15 0,-9-33 0,-1-3 0,-18-9 0,13-10 0,-26-4 0,13-3 0,-15-2 0,4-4 0,-5-1 0,0-4 0,0-9 0,13-16 0,10-13 0,25-31 0,-21 32 0,2-2-803,5-11 0,3-3 803,7-5 0,4-3-1093,-7 5 1,3-4 0,0 0 1031,0 0 0,1-1 0,3-2-759,-6 7 1,3-3 0,1-1 0,0-2 598,1-3 0,0-2 0,1-2 1,4-4-327,-7 9 1,3-2 0,3-3 0,1-2 0,0-1 0,-1 0 481,-5 5 1,-1-1-1,1-1 1,0 0 0,1-2-1,1-2 1,2-1-166,-5 6 1,1-2-1,2-1 1,1-1 0,0-1-1,1-1 1,0 0 0,1-1-1,-1 1 230,-2 3 0,2-2 0,0 0 0,0-1 0,1 0 0,0 0 0,-1 1 0,-1 1 0,-1 1 0,-2 2-124,5-6 0,-2 2 1,-1 1-1,0 1 1,-1 1-1,-1 0 0,2 1 1,-1-1 123,9-10 0,2-1 0,0 0 0,-1 1 0,-1 3 0,-4 4 0,-5 6-3,7-7 0,-5 7 1,-2 3-1,1-2 3,6-6 0,0-1 0,1 1 0,-2 4 0,9-6 0,-1 5 0,0-1 287,-14 13 1,1-1-1,-1 1 1,-2 5-288,2 1 0,-2 5 0,-1 5 1268,15-2 1,-5 10-1269,6 2 0,11 64 0,-58 12 0,-8 14 0,5 35 0,-4 2 0,-5-33 0,-1-3 0,-4 0 0,-1 1 0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink19.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2021-08-25T14:03:34.471"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.2" units="cm"/>
+      <inkml:brushProperty name="height" value="0.2" units="cm"/>
+      <inkml:brushProperty name="color" value="#008C3A"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">0 3658 24575,'0'60'0,"0"19"0,14 18-1440,-2-39 1,1 2 1439,3 9 0,3 1 0,8-7 0,-1-3 297,-15-8 0,0-2-297,35 34 0,-29-18 0,9-7 546,-3-1-546,-10-24 0,2-13 0,-5-2 1475,-1-4-1475,1 0 264,-1-1-264,0-5 0,5 1 0,2 4 0,4-3 0,-5 3 0,4-4 0,-9 0 0,4-5 0,0-1 0,-3-4 0,3 0 0,0 0 0,1-4 0,5-2 0,0-4 0,6-5 0,2 3 0,5-9 0,8-4 0,13-22 0,-16 10 0,1-5-1639,7-18 1,3-10 1480,-11 12 0,2-5 1,2-5-1,-1-1-662,5-9 1,-1-3 0,1-4 0,1-4 450,-7 13 0,1-6 1,0-2-1,1-1 0,-1 2 1,-1 2-288,3-3 1,-1 2-1,0 1 1,-1 1 0,-1-2 634,-2 1 0,-1 0 0,0 0 1,1 0-1,1 2 21,0 3 0,2 0 0,1 1 0,-1 2 0,0 0 0,5-10 0,-2 2 0,2 0 0,3-2 0,-2 7 0,3-1 0,1-1 0,1 1 0,-2 3 0,6-7 0,-1 3 0,1 3 0,0 2-399,-1 7 1,1 3 0,0 2 0,1 3 398,12-12 0,0 4 0,1 3 0,2 5 0,1 3 0,-1 2 361,-6 5 0,-1 3 1,2 1-362,10-1 0,3 1 0,-5 3 0,8-6 0,-4 2 1425,4 0 1,-5 4-1426,-27 16 0,-5 2 0,19-22 3276,-8 23-2143,-29 0 2143,-7 12-2784,-7 5 412,-5 1-904,0 4 338,0 0 1,-4 0 0,-2 0 0</inkml:trace>
+</inkml:ink>
+</file>
+
 <file path=xl/ink/ink2.xml><?xml version="1.0" encoding="utf-8"?>
 <inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
   <inkml:definitions>
@@ -1488,6 +2823,286 @@
 </inkml:ink>
 </file>
 
+<file path=xl/ink/ink20.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2021-08-25T14:02:25.376"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+      <inkml:brushProperty name="color" value="#E71224"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">0 55 24575,'96'6'0,"-1"0"0,0 0 0,0-1 0,1 1 0,-1 0 0,0 0 0,0 0 0,0-1 0,1 1 0,-1 0 0,0 0 0,0-1 0,-2 5 0,-17-1 0,-5 0 0,5 0 0,17 1 0,-16-4 0,13 1 0,9-1 0,7 1 0,6 0 0,2-1 0,0 1 0,-1-1 0,-5 1 0,-7-1 0,-9 0 0,-11-1 0,-14 1 0,33 5 0,-22-1 0,-12-4 0,24-6-1680,-1 0 1,-8 0 1679,-35 0 784,49 0-784,-54 0 0,57 0 0,-27 0 0,-4 0-2002,-3 0 2002,4 0 0,1 0 0,10 0 0,-29 0 0,19 0 2287,7 0-2287,-36 0 0,29 0 0,8 0 0,-18 0 0,-9 0 0,3 0 0,0 0 0,-2 0 0,18 0 2290,9 0-2290,1 0 0,-43 0 0,26 0 0,-20 0 0,-11 0 0,18 0 0,8 0 0,-2 0 0,-1 0 0,42 0 0,-56 0 0,39 0 0,-19 0 0,-2 0 0,1 0 0,-1 0 0,2 0 0,19 0 0,-30 0 0,20 0 0,-41 0 0,0-5 0,-12 3 0,48-17 0,-41 16 0,42-22 0,-45 22 0,8-13 0,38 4 0,-26 5 0,39-11 0,-39 11 0,-11-4 0,28-5 0,-35 9 0,33-8 0,11 2 0,-31 5 0,27-4 0,20 0 0,-51 4 0,65-5 0,-47-1 0,15 3 0,0-1 0,-4-3 0,-21 14 0,11 23 0,-14 2 0,7 26 0,-1 0 0,-19-18 0,12 16 0,4 10 0,-24-21 0,19 18 0,-25-8 0,-7-12 0,8 15 0,-10 6 0,0-30 0,0 30 0,0-6 0,0-19 0,0 11 0,0-19 0,0-11 0,0 11 0,0 19 0,0-25 0,0 39 0,0-30 0,0 13 0,0-13 0,0 11 0,0-25 0,0 14 0,0-12 0,-4 4 0,3-4 0,-3 3 0,0-3 0,-3 14 0,2-12 0,-1 7 0,6 19 0,0-25 0,0 25 0,-10 1 0,8-13 0,-15 20 0,15-13 0,-6-20 0,4 9 0,3-2 0,-7-8 0,7 20 0,-3-10 0,0 4 0,3-6 0,-3-7 0,4-3 0,0-1 0,-34 42 0,25-36 0,-25 32 0,34-42 0,0 4 0,0-3 0,-9 36 0,7-25 0,-8 22 0,1 3 0,7-7 0,-19 22 0,18-23 0,-9-14 0,12 22 0,-4-29 0,3 30 0,-3-37 0,4 6 0,0-2 0,-4 4 0,3-4 0,-3 3 0,0-3 0,-5 4 0,3 0 0,-6 0 0,11 0 0,-3-4 0,4-1 0,0 9 0,-4-9 0,3 9 0,-9 1 0,9-7 0,-5 8 0,0 2 0,1-13 0,-8 23 0,7-24 0,1 11 0,1-14 0,3 4 0,-7 1 0,7 0 0,-3 3 0,4-7 0,-8 7 0,6 6 0,-6-6 0,8 5 0,0-9 0,-13 70 0,10-52 0,-10 50 0,13-68 0,-4-3 0,3 3 0,-3-4 0,4 4 0,0-3 0,-4 7 0,3-3 0,-3 0 0,0 3 0,-1-7 0,0 3 0,1-4 0,4 0 0,0-1 0,-4 5 0,3-3 0,-3 3 0,4-4 0,0 4 0,-4 1 0,3 0 0,-3 3 0,4-3 0,0 0 0,-4 3 0,3-7 0,-3 36 0,4-29 0,0 26 0,-9-1 0,3-25 0,-5 25 0,3-29 0,7-3 0,-3 3 0,4-4 0,0 4 0,0-3 0,-4 7 0,3-3 0,-3 0 0,4-1 0,0 0 0,-5 10 0,3-6 0,-22 39 0,19-39 0,-14 29 0,15-32 0,3 0 0,-8 13 0,7-15 0,-4 10 0,2-13 0,3 0 0,-3 53 0,4-36 0,0 37 0,-6-36 0,1-11 0,-10 8 0,1-15 0,-4-9 0,0-5 0,4-4 0,1 0 0,2-14 0,6 11 0,-1-15 0,6 13 0,-23-53 0,10 37 0,-16-33 0,16 47 0,3-33 0,1-5 0,-2 19 0,2-20 0,-1 8 0,1 38 0,4 1 0,1-5 0,4-1 0,18 4 0,-10 6 0,19 13 0,-21 5 0,2 0 0,4 12 0,-10-14 0,14 11 0,-15-10 0,11 1 0,-6 0 0,7-1 0,-8-4 0,-1 0 0,0 0 0,1 4 0,4-3 0,0 7 0,47 52 0,-35-41 0,35 45 0,-46-50 0,-4-2 0,4 6 0,-5-13 0,0 3 0,3-7 0,-7 3 0,-1-4 0,-1-12 0,-3-3 0,4-12 0,0 4 0,0-3 0,0 3 0,8-4 0,2 1 0,8 3 0,-4 1 0,-2 4 0,1 0 0,-3 0 0,7-4 0,-7 3 0,3-3 0,-4 4 0,4-4 0,-3 7 0,3-6 0,0 3 0,1-5 0,0 0 0,3 1 0,-7 4 0,3 4 0,-4 1 0,0 0 0,0-1 0,-4 0 0,-1 1 0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink21.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2021-08-25T14:02:25.384"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+      <inkml:brushProperty name="color" value="#E71224"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 1 24575,'13'0'0,"1"0"0,0 0 0,12 0 0,20 0 0,38 0 0,-15 0 0,10 0 0,-1 0 0,-38 0 0,27 0 0,-49 0 0,-4 0 0,3 0 0,-3 0 0,0 0 0,3 0 0,-7 0 0,36 0 0,-25 0 0,36 0 0,-37 0 0,17 0 0,-7 0 0,0 0 0,-6 0 0,42 23 0,-44-18 0,25 10 0,1 2 0,-27-6 0,55 0 0,-54 1 0,53-2 0,-58-4 0,59 13 0,-59-17 0,25 8 0,-29-6 0,-3 1 0,7 4 0,-7-4 0,17 10 0,-15-8 0,7 14 0,-7-7 0,-2 4 0,3-4 0,4 3 0,-11-3 0,6 0 0,-7-1 0,19 29 0,-4-11 0,6 14 0,21 19 0,-35-44 0,26 34 0,-33-40 0,4 0 0,-4-1 0,3 0 0,1 1 0,1 4 0,-1 0 0,-1-4 0,5 12 0,-6-9 0,4 6 0,-5 4 0,0-11 0,1 41 0,1-36 0,-7 21 0,3-29 0,-4-3 0,0 7 0,0-3 0,0 4 0,0-4 0,0 3 0,0 7 0,0-4 0,0 4 0,0 22 0,0-29 0,0 29 0,0-22 0,0-8 0,0 20 0,0-23 0,0 9 0,0-13 0,0 14 0,0-11 0,0 11 0,0-1 0,0-9 0,0 9 0,0-9 0,0 1 0,0 0 0,0 13 0,0-15 0,0 11 0,0-1 0,0-6 0,0 12 0,0-10 0,0-4 0,0 3 0,0 6 0,0-2 0,0 2 0,0-6 0,0 7 0,0-8 0,0 40 0,0-39 0,0 39 0,0-30 0,0 4 0,4-2 0,1-15 0,-1 14 0,4-11 0,-7 12 0,3-1 0,-4-6 0,0 6 0,0-13 0,4 3 0,-3-3 0,3 4 0,-4 0 0,0 29 0,0-25 0,0 20 0,0-20 0,0 4 0,0 4 0,0-6 0,0-7 0,0-3 0,0 0 0,0 3 0,0-3 0,0 0 0,0-2 0,0-3 0,0 4 0,0 1 0,0 0 0,0 3 0,0-3 0,0 0 0,0 3 0,0-7 0,0 7 0,0-3 0,0 0 0,0 3 0,0-3 0,0 0 0,0 3 0,0-3 0,0 0 0,0-1 0,0 9 0,0-9 0,0 13 0,0-2 0,0-4 0,0 8 0,0-10 0,0-4 0,0 12 0,0-14 0,0 11 0,0-10 0,0-3 0,0 7 0,0-3 0,0 4 0,0 9 0,0 3 0,0 10 0,0-10 0,0-3 0,0-9 0,0-4 0,0 3 0,0-3 0,0 14 0,0-12 0,0 7 0,0-14 0,0 4 0,0-3 0,0 3 0,0-5 0,0 5 0,0-3 0,0 3 0,0 30 0,0-22 0,-5 36 0,-1-41 0,-9-5 0,5-13 0,1-11 0,1 0 0,3 3 0,-4-7 0,-5-26 0,4 17 0,0-17 0,6 30 0,4 4 0,0-4 0,0 3 0,0-7 0,0 3 0,-8-4 0,2 0 0,-3 4 0,5 2 0,0 3 0,3 8 0,-3 6 0,4 9 0,0-1 0,11 14 0,-8-15 0,13 15 0,-15-17 0,9 16 0,-9-13 0,5 9 0,-6-9 0,4 1 0,1 0 0,4 3 0,0-7 0,-4 3 0,-1-4 0,0 4 0,-3-3 0,21 11 0,-14-14 0,28 16 0,-10-26 0,0 9 0,4-30 0,-23 12 0,5-11 0,-8 10 0,-3 3 0,7-3 0,-7 0 0,7-1 0,-7 0 0,11-3 0,-4-6 0,1 2 0,1-2 0,-9 10 0,3 4 0,0-4 0,-3 3 0,7-7 0,-3 7 0,0-7 0,-1 7 0,0-3 0,-3 4 0,7-4 0,-3 3 0,4-3 0,-4 8 0,-1 1 0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink22.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2021-08-25T14:02:25.385"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+      <inkml:brushProperty name="color" value="#E71224"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">3156 0 24575,'-9'4'0,"-41"31"0,26-22 0,-31 21 0,27-34 0,8 4 0,-8-3 0,14 3 0,1-4 0,1 0 0,2 0 0,-17 0 0,15 0 0,-15 0 0,4 0 0,6 0 0,-5 0 0,-21 0 0,26 0 0,-29 0 0,22 0 0,4 0 0,-4 0 0,8 0 0,2 0 0,0 0 0,1 0 0,4 0 0,-4 0 0,-11 0 0,-6 0 0,4 0 0,-10 0 0,24 0 0,-11 0 0,-19 0 0,25 0 0,-26 0 0,1 0 0,25 0 0,-29 0 0,22 0 0,4 0 0,-4 0 0,-41 0 0,42 0 0,-38 0 0,48 0 0,3 0 0,-7 0 0,3 0 0,-4 0 0,-10 0 0,12 0 0,-7 0 0,1 0 0,5 0 0,-6 0 0,6 0 0,-7 0 0,4 0 0,-8 0 0,1 0 0,11 0 0,-7 0 0,-19 0 0,24 0 0,-24 0 0,0 0 0,11 0 0,-14 0 0,-11 0 0,25 0 0,-28 0 0,33 0 0,-50 34 0,54-25 0,-53 25 0,62-34 0,-9 0 0,-20 0 0,24 0 0,-37 0 0,42 0 0,-23 0 0,20 0 0,-8 0 0,-22 18 0,29-13 0,-39 19 0,40-14 0,-8 2 0,11-3 0,4-5 0,0 0 0,-13 3 0,9-2 0,-25 21 0,-6 5 0,6-7 0,-30 34 0,31-20 0,6 1 0,9 18 0,-32 20 0,45-35 0,5-33 0,-9 13 0,7-9 0,-10 9 0,15-9 0,-7-3 0,1 17 0,-11 58 0,9-45 0,-3 20 0,2-5 0,7-38 0,-6 29 0,9-32 0,0 0 0,0-1 0,-4-4 0,3 4 0,-3-3 0,4 3 0,0 10 0,-4-7 0,-5 12 0,3-14 0,-2-1 0,8-4 0,0 0 0,0 13 0,-6 4 0,5 14 0,-5-14 0,6 0 0,0-2 0,0-4 0,0 4 0,0-7 0,0-3 0,0 0 0,0-2 0,0 11 0,0-11 0,0 11 0,0-14 0,-6 14 0,5-11 0,-5 10 0,6-9 0,0-3 0,0 56 0,0-44 0,0 40 0,0-49 0,0-3 0,0 3 0,0-4 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 4 0,0-3 0,0 3 0,0-4 0,0 13 0,0-9 0,0 9 0,0-9 0,0-3 0,0 36 0,0-28 0,0 24 0,0-33 0,-4 0 0,3 4 0,-3 50 0,4-37 0,0 36 0,0-50 0,0-2 0,0 3 0,0 49 0,0-40 0,0 44 0,0-56 0,0 3 0,0-4 0,0 4 0,-8 1 0,6 0 0,-6 3 0,4-7 0,3 3 0,1-4 0,1-8 0,3 2 0,-4-7 0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink23.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2021-08-25T14:02:25.386"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+      <inkml:brushProperty name="color" value="#E71224"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">0 214 24575,'79'0'0,"-30"0"0,20 0 0,-12 0 0,-22 0 0,11 0 0,-20 0 0,-12 0 0,4 0 0,10 0 0,-12 0 0,11 0 0,-4 0 0,-3 0 0,8 0 0,0 0 0,-8 0 0,7 0 0,1 0 0,-12 0 0,11 0 0,-4 0 0,-6 0 0,5 0 0,1 0 0,-11 0 0,24 0 0,-19 0 0,20 0 0,-17 0 0,4 0 0,42 0 0,-31 0 0,35 0 0,6 0 0,-36 0 0,25 0 0,-9 0 0,-35 0 0,26 0 0,-19 0 0,-8 0 0,8 0 0,19 0 0,-12 0 0,14 0 0,28 0 0,-47 0 0,37 0 0,-1 0 0,-31 0 0,42 0 0,-57 0 0,17 0 0,-25 0 0,10 0 0,-13 0 0,34 0 0,-26 0 0,78 0 0,-59 0 0,33 0 0,-10 13 0,-2 1 0,-8-7 0,8 7 0,4-1 0,38-13 0,-25 0 0,19 0 0,3 0 0,-17 0 0,10 0 0,-20 0 0,0 0 0,4 0 0,21 0 0,-23 0 0,-7 0-2085,-24 0 2085,30 0 0,-4 0 0,-41 0 0,71 12 0,-56-9 0,29 8 0,7-11 0,-36 0 0,29 0 0,8 0 0,-18 0 0,15 0 0,-4 0 0,-5 0 0,-25 0 1042,25 0 1,6 0-1043,22 0 0,-19 0 0,15 0 0,-18 0 0,-7 0-2978,-19 0 2978,38 0 0,9 0 0,-31 0 0,-4 0-1972,41 0 1972,-38 0 0,-1 0 0,19 0 0,-28 0 0,28 0 0,1 0 0,-10 0 0,5 0 0,22 0 2643,-48 0-2643,12 0 0,0 0 0,-2 0 2307,7 0-2307,30 0 0,-64 0 0,55 0 0,1 0 0,-43 0 0,45 0 0,-20 0 0,-3 0 0,9 0 0,-11 0 0,5 0 0,1 0 0,-5 0-540,4 0 540,1 0 0,3 0 0,-20 0 0,-3 0 0,39 0 0,-19 0 0,-11 0 0,-4 0 0,-14 0 0,44 0 0,-10 0 0,-39 0 0,33 0 0,-12 0 540,-36 0-540,35 0 0,-40 0 0,41 0 0,-36 0 0,35 0 0,-43 0 0,9 0 0,-9 0 0,-3 0 0,7 0 0,-7 0 0,3-4 0,0 3 0,1-7 0,4 7 0,0-3 0,42-3 0,5 0 0,-24 3 0,22-4 0,-5 2 0,-35 6 0,-11 0 0,10 0 0,1-6 0,-11 4 0,11-4 0,-14 6 0,14 0 0,-11-4 0,44-6 0,-39 4 0,25-4 0,-29 6 0,-3 3 0,36-2 0,-28 3 0,24-4 0,-20 3 0,-5-3 0,-2 4 0,-16 0 0,-13 0 0,0 0 0,-12-6 0,13 4 0,-9-4 0,-1-5 0,7 8 0,-8-9 0,11 12 0,0 0 0,-20-28 0,18 17 0,-17-26 0,27 27 0,-4-7 0,0 7 0,10-16 0,33 27 0,-11-13 0,25 31 0,-21-2 0,-10 2 0,5-1 0,-13-5 0,24 20 0,-18-14 0,18 15 0,-24-25 0,30 40 0,-23-38 0,27 39 0,-29-45 0,4 8 0,-12-3 0,-16 5 0,-27 18 0,-5-14 0,-47 21 0,40-19 0,-20-3 0,45-5 0,-3-3 0,15-9 0,-10 13 0,13-8 0,4 7 0,-3-4 0,7-4 0,-3-1 0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink24.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2021-08-25T14:02:25.387"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+      <inkml:brushProperty name="color" value="#E71224"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">0 416 24575,'55'0'0,"2"0"0,-37 0 0,17 0 0,32 0 0,-29 0 0,27 0 0,-20 9 0,-26-6 0,35 6 0,-30-9 0,53 11 0,-43-4 0,25 5 0,-18-8 0,-13-4 0,16 0 0,29 0 0,-48 0 0,39 0 0,1 0 0,-37 0 0,37 0 0,-20 0 0,-12 0 0,11 0 0,29 0 0,-39 0 0,29 0 0,11 12 0,-50-9 0,50 8 0,-55-11 0,55 0 0,-36 0 0,29 0 0,-32 0 0,-21 0 0,21 0 0,-25 0 0,44 0 0,-39 0 0,29 0 0,-22-6 0,-8 5 0,20-11 0,-19 11 0,10-9 0,-9 9 0,0-7 0,10 7 0,41-37 0,-29 29 0,26-25 0,-52 34 0,3-4 0,-3 3 0,4-3 0,-4 4 0,32 0 0,-28 0 0,37 0 0,-9 0 0,-15-4 0,15 3 0,-22-3 0,-8 4 0,6 0 0,-9 0 0,-3 0 0,3 0 0,10 0 0,-11 0 0,15 0 0,-4 0 0,-6 0 0,19 0 0,-20 0 0,8 0 0,2 0 0,-13 0 0,43 0 0,-39 0 0,25 0 0,0 0 0,-11 0 0,19 0 0,-13 0 0,-17 0 0,4 0 0,-7 0 0,-7 0 0,3 0 0,-4 0 0,4 0 0,-3 0 0,6 0 0,-2 0 0,4 0 0,-4 0 0,33 0 0,-30 0 0,29 0 0,-36 0 0,3 0 0,0 0 0,1 0 0,0 0 0,-1 0 0,29 0 0,-25 0 0,39 0 0,-44 0 0,11 0 0,-14-4 0,0-1 0,0 0 0,0 1 0,13 4 0,-9 0 0,13 0 0,-12 0 0,0 0 0,-1 0 0,-4 0 0,4 0 0,-3 0 0,3-4 0,-4 3 0,4-3 0,11-2 0,-4 5 0,3-5 0,-10 6 0,-4 0 0,4 0 0,-3 0 0,7 0 0,-3 0 0,0 0 0,3 0 0,-3 0 0,4 0 0,29 0 0,-26 0 0,35 0 0,-43 0 0,23-6 0,-24 5 0,11-5 0,-14 2 0,0-1 0,0 0 0,0 1 0,0 4 0,0 0 0,4 0 0,-4 0 0,4 0 0,0 0 0,11 0 0,-8 0 0,7 0 0,-1 0 0,-9 0 0,1 4 0,-15-7 0,-8 2 0,4-8 0,1 0 0,4-4 0,0 3 0,0-3 0,0 0 0,0 3 0,0-3 0,0 4 0,6-13 0,0 9 0,5-9 0,-2 13 0,23-24 0,-17 18 0,32-20 0,-31 22 0,8 5 0,-7-4 0,-7 11 0,3-3 0,-4 4 0,4 0 0,-3 0 0,3 0 0,-4 0 0,4 0 0,-4 0 0,4 0 0,10 0 0,-11 0 0,15 0 0,-3 0 0,-8 0 0,6 0 0,1 0 0,-7 4 0,12-3 0,-14 7 0,-1-7 0,-4 3 0,0 0 0,0-3 0,0 3 0,0 0 0,0-3 0,13 14 0,-9-12 0,42 28 0,-24-15 0,15 10 0,-24-10 0,-13-11 0,0 3 0,42 39 0,-36-28 0,15 32 0,-3 1 0,-20-29 0,5 42 0,-8-55 0,-4 3 0,0-4 0,0 0 0,0 0 0,0 0 0,4 0 0,5 0 0,1-4 0,7-1 0,-3-4 0,14 0 0,21 0 0,-14 0 0,12 0 0,0 0 0,-12 0 0,11 0 0,10 0 0,-39 0 0,25 0 0,0 0 0,-25 0 0,39 0 0,9 0 0,-29 0 0,30 0 0,-3 0 0,-23 0 0,29 0 0,7 0 0,-36 0 0,29 0 0,-9 0 0,-4 0 0,-16 0 0,19 0 0,-3 0 0,-26 0 0,30 0 0,-16 0 0,15 0 0,20 0 0,-30 0 0,21 0 0,6 0 0,-36 0 0,29 0 0,7 0 0,-36 0 0,29 0 0,-12 0 0,-36 0 0,35 0 0,-39 0 0,10 0 0,-9 0 0,-4 0 0,32 0 0,-29 0 0,30 0 0,-33 0 0,0 0 0,2 0 0,16 0 0,-14 0 0,66 0 0,-62 0 0,53 0 0,-9 0 0,-27 0 0,24 0 0,3 0 0,-30 0 0,29 0 0,-9 0 0,-39 0 0,25 0 0,-19 0 0,-11 0 0,24 0 0,-10 0 0,4 0 0,-2 0 0,38 0 0,-39 0 0,48 0 0,-29 0 0,-15 0 0,15 0 0,-3 0 0,-22 0 0,25 0 0,17 0 0,-37 0 0,69 0 0,-25 0 0,-1 0 0,10 0 0,0 0 0,-10 0 0,5 0 0,22 0 0,-70 0 0,50 6 0,-31 5 0,-10-3 0,8 1 0,23 3 0,-40-10 0,41 10 0,-39-12 0,-12 0 0,11 0 0,-4 0 0,-2 4 0,6-3 0,1 3 0,-8-4 0,4 0 0,41 0 0,-42 0 0,72 0 0,-25 0 0,-11 0 0,17 0 0,13 0 0,-26 6 0,8-6 0,-3 1 0,-24 5 0,31-6 0,-58 0 0,20 0 0,-17 4 0,17 3 0,-20-2 0,5 5 0,1-9 0,-7 3 0,12-4 0,-10 0 0,-4 0 0,3 0 0,-3 0 0,0 0 0,2 0 0,-2 0 0,0 4 0,13-3 0,-11 3 0,21-4 0,-20 0 0,39 9 0,-39-6 0,25 6 0,-19-9 0,-7 8 0,21 0 0,-20 1 0,19-3 0,-10-6 0,4 0 0,-3 0 0,20 19 0,-21-15 0,21 15 0,20-19 0,-41 0 0,49 12 0,-59-9 0,12 8 0,0-5 0,-8-4 0,7 3 0,-13-5 0,3 0 0,7 6 0,-8-4 0,20 4 0,-23-6 0,9 0 0,1 6 0,-11-5 0,24 17 0,-10-10 0,14 11 0,39 0 0,-43-10 0,39 14 0,-49-20 0,14 9 0,-1-7 0,-9-3 0,7 4 0,-7-6 0,0 4 0,7-3 0,-16 7 0,35 11 0,-1-1 0,29 12 0,-34-18 0,-8-3 0,20-9 0,-36 4 0,41-3 0,-20 22 0,-26-18 0,22 17 0,-34-21 0,0 7 0,0-7 0,0 3 0,0-4 0,-1 0 0,15 6 0,-7 3 0,12-1 0,-10 0 0,-4-4 0,3-3 0,-3 7 0,0-7 0,40 37 0,-34-25 0,34 26 0,-44-34 0,7 7 0,-7-6 0,3 7 0,-4-4 0,0 0 0,0 0 0,0 0 0,4 4 0,-3-3 0,7 7 0,-3-3 0,-1-1 0,4 4 0,-7-3 0,3 0 0,-4-1 0,0 0 0,0-3 0,-4 7 0,7-3 0,-6 0 0,7-1 0,1 29 0,-3-24 0,3 28 0,-9-36 0,-1 3 0,-4 9 0,0-9 0,0 9 0,0-9 0,0-3 0,0 3 0,0 10 0,0-7 0,0 8 0,0-8 0,0-6 0,0 3 0,0 10 0,-4-11 0,-1 11 0,-4-14 0,-4 4 0,3-3 0,-3 3 0,-9-2 0,13 2 0,-12 3 0,20 31 0,-9-12 0,8 10 0,-4-18 0,6-17 0,0 7 0,0-7 0,-4 7 0,3 6 0,-2-6 0,-9 19 0,0-65 0,-6 29 0,3-47 0,-1 20 0,-3-3 0,0 4 0,7 3 0,-11-19 0,14 25 0,-14-29 0,14 32 0,4 0 0,-7-3 0,6 3 0,-11-4 0,11 4 0,-2 9 0,8 19 0,4 3 0,1 6 0,8-6 0,-3-7 0,-1 3 0,-1-4 0,-1 14 0,16-15 0,-5 14 0,9-17 0,-13 8 0,3-3 0,-3 3 0,4-4 0,-4-4 0,13-1 0,-1 1 0,0 1 0,-4 5 0,1 0 0,-7-6 0,12 1 0,-10-14 0,-4 2 0,3-7 0,-7 4 0,3 4 0,9-11 0,-10 9 0,11-9 0,-14 7 0,4-4 0,-3 7 0,3-2 0,-4 4 0,0-1 0,0 0 0,24-27 0,-18 21 0,31-30 0,-38 34 0,10-4 0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink25.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2021-08-25T14:02:25.388"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+      <inkml:brushProperty name="color" value="#E71224"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">0 130 24575,'9'0'0,"0"0"0,4 0 0,1 0 0,13 0 0,-10 0 0,5 0 0,-13 0 0,14 0 0,-11 0 0,24 0 0,-23 0 0,9 0 0,1 0 0,-11 0 0,11 0 0,-14 0 0,13 6 0,-9-4 0,23 4 0,-24-6 0,11 0 0,19 18 0,-25-13 0,26 13 0,-1-18 0,-25 4 0,29-3 0,-22 3 0,6 2 0,-4-4 0,-4 4 0,-9-6 0,-3 0 0,3 0 0,0 4 0,-3-3 0,7 3 0,7-4 0,-8 0 0,10 7 0,-16-5 0,17 6 0,-15-8 0,25 6 0,-25-4 0,10 4 0,-9-6 0,-3 0 0,7 0 0,-3 0 0,4 4 0,10-3 0,-12 3 0,40-4 0,-39 0 0,29 0 0,-22 0 0,-8 0 0,7 0 0,-1 0 0,-9 0 0,9 0 0,1 0 0,-11 0 0,11 0 0,-10 0 0,1 0 0,0 0 0,3 0 0,-3 0 0,0 0 0,3 0 0,-3 0 0,-1 0 0,4 0 0,-3 0 0,14 0 0,-12 0 0,7 0 0,-14 0 0,4 0 0,1 0 0,0 0 0,-1 0 0,9 0 0,-9 0 0,13 0 0,-12 0 0,0 0 0,3 0 0,-7 0 0,3 0 0,0 0 0,-3 0 0,7 0 0,-7 0 0,7 0 0,-3 0 0,0 0 0,36 0 0,5 0 0,-19 0 0,17-1 0,-4-2 0,-32-2 0,-7 0 0,3-3 0,9 7 0,-9-3 0,9 4 0,-13-4 0,4 3 0,-3-3 0,3 0 0,-4 3 0,14-9 0,-11 4 0,10-4 0,21 5 0,-12-5 0,14 8 0,11-13 0,-39 13 0,25-11 0,-33 8 0,4 0 0,-3 1 0,7 0 0,-7-1 0,7 0 0,-7 1 0,3 4 0,29-10 0,-24 8 0,28-7 0,-32 5 0,0-1 0,3 0 0,-7 1 0,2 4 0,-3 0 0,4 0 0,-3 0 0,3 0 0,-4 0 0,4 0 0,-3 0 0,3 0 0,-4 0 0,14-6 0,-11 4 0,11-3 0,-10 5 0,1 0 0,0 0 0,3 0 0,-8 0 0,8 0 0,-3 0 0,0 0 0,-1 0 0,-4 0 0,4 0 0,1 0 0,0 0 0,3 0 0,7 0 0,-4 0 0,4 0 0,-7 0 0,-8 0 0,4 0 0,0 0 0,-3 0 0,7 0 0,-7 0 0,3 0 0,-4 0 0,4 0 0,1 0 0,0 0 0,3 0 0,-3 0 0,0 0 0,3 0 0,-7 0 0,3 0 0,9 0 0,-9-4 0,9 3 0,-13-3 0,4 4 0,1 0 0,0 0 0,13-6 0,-11 4 0,12-4 0,-14 2 0,-1-1 0,9 0 0,-9 1 0,9 4 0,-9-4 0,-3 3 0,3-3 0,-4 4 0,0 0 0,4 0 0,69 0 0,-51-3 0,64 2 0,-78-3 0,6 4 0,-6 0 0,-7 0 0,7 0 0,-3 0 0,0 0 0,-1 0 0,-4 0 0,4 0 0,-3 0 0,3 0 0,10 0 0,-11 0 0,44 0 0,-35 7 0,26-1 0,-33 3 0,13-5 0,-15 0 0,15 1 0,-17 4 0,6 4 0,-6-7 0,3 6 0,23 21 0,2 4 0,-17-8 0,19 12 0,-7-3 0,-32-24 0,12 32 0,-11-29 0,14 39 0,-15-44 0,17 24 0,-16-23 0,10 13 0,-12-12 0,0 4 0,6 10 0,-4-8 0,3 4 0,-5 22 0,0-29 0,0 39 0,0-11 0,0-14 0,0 16 0,0-4 0,0-22 0,0 25 0,0-32 0,0 0 0,0 13 0,0-15 0,0 11 0,0-11 0,0 12 0,0-4 0,0 8 0,0-14 0,0 3 0,0-3 0,0 0 0,0 12 0,0-9 0,0 10 0,0-13 0,0 3 0,0-3 0,0 0 0,0 3 0,0-3 0,0 0 0,0 32 0,0-25 0,0 23 0,0 2 0,0-29 0,0 29 0,0-22 0,0-4 0,0 4 0,0-7 0,0-3 0,0 0 0,0-2 0,0 31 0,0-22 0,0 26 0,0-33 0,0 3 0,0-3 0,0 0 0,0-1 0,0-4 0,0 4 0,0-3 0,0 3 0,0-4 0,0 13 0,0-5 0,0 10 0,0-13 0,0 3 0,0 7 0,0-4 0,0 8 0,0-14 0,0-2 0,0 11 0,0-11 0,0 11 0,0-14 0,0 4 0,0-3 0,0 7 0,0-3 0,0 0 0,0-1 0,0 29 0,0-25 0,0 25 0,0-29 0,0 1 0,0 0 0,0 3 0,0-3 0,0 0 0,0 3 0,0-7 0,0 3 0,0-4 0,0 14 0,0-11 0,0 24 0,0-20 0,0 8 0,0 3 0,0-15 0,0 10 0,0 1 0,0 23 0,0-16 0,0 13 0,0-21 0,0-9 0,0 9 0,0-13 0,0 53 0,0-36 0,0 37 0,0-50 0,0-4 0,0 4 0,0-3 0,0 3 0,0-4 0,0 4 0,0-3 0,0 55 0,0-38 0,0 27 0,-4-51 0,-1-12 0,0-13 0,-3 10 0,-1-11 0,-8 0 0,2 11 0,-2-15 0,4 14 0,7-5 0,-6 4 0,11-3 0,-7 7 0,7-3 0,-7 4 0,3 0 0,-4-4 0,-34-70 0,22 52 0,-16-46 0,48 85 0,5 3 0,23 39 0,-15-15 0,1 11 0,-8-24 0,-8-13 0,-4 4 0,-1-3 0,0 3 0,5 0 0,-3-3 0,6 7 0,-7-7 0,0 7 0,27 17 0,-21-15 0,22 14 0,-28-32 0,-1-6 0,-4-5 0,0-17 0,0 11 0,8-12 0,-2 10 0,3 5 0,-5-4 0,1-7 0,-3 8 0,8-7 0,-9 1 0,3 9 0,0-9 0,5 9 0,1-1 0,3 0 0,-4 1 0,4 0 0,-3 3 0,3-3 0,-5 4 0,34-26 0,4-4 0,-22 18 0,18-13 0,-1 0 0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink26.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2021-08-25T14:02:25.389"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+      <inkml:brushProperty name="color" value="#E71224"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">0 197 24575,'9'-5'0,"14"1"0,-7 4 0,12 0 0,38 0 0,-26 0 0,39 0 0,-20 0 0,1 0 0,3 0 0,36 0-379,-30 0 1,4 0 378,9 0 0,-2 0-2299,-19 0 0,1 0 2299,28 0 0,7 0 0,-21 0 0,2 0 0,-6 0 0,-6 0 0,1 0 0,3 0 0,6 0 0,-1 0 0,-4 0 0,-1 0 0,-5 0-631,1 0 0,1 0 631,4 0 0,7 0 0,-6 0 0,5 0 0,-7 0 0,-10 0 0,-1 0 0,11 0 0,2 0 0,1 0 0,-3 0 0,28 0 0,-38 0 0,3 0 0,9 0 0,-6 0 0,-7 0 0,-1 0 0,2 0 0,19 0 0,-30 0 0,20 0 0,-9 0 0,-4 0 0,-16 0 266,16 0 0,4 0-266,9 0 0,-29 0 4375,36 0-4375,-7 0 0,-29-4 1710,27 3-1710,-20-3 0,-12-2 0,10 4 0,11-4 0,-25-5 0,15 8 0,-10-9 0,-20 12 0,12-4 0,23 3 0,-15-3 0,13 4 0,-26 0 0,19 0 0,-21 0 0,36-6 0,-41 5 0,21-5 0,-25 6 0,10-4 0,-13 3 0,0-7 0,-8 3 0,-2 0 0,-12-7 0,3 10 0,-2-10 0,3 11 0,0-3 0,-4 0 0,3-1 0,-3 0 0,4 1 0,0 4 0,0 0 0,0-4 0,0 3 0,0-3 0,0 4 0,0 0 0,-4 0 0,3 0 0,-7-4 0,3 3 0,0-3 0,1 4 0,4 0 0,-4 0 0,3 0 0,-7 0 0,3 0 0,-4 0 0,4 0 0,-2 0 0,6 0 0,-3 0 0,12-4 0,2 3 0,8-7 0,4 3 0,-4 0 0,4 1 0,-4 4 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,4 0 0,-3 0 0,3 0 0,29 10 0,-24-4 0,24 8 0,-33-5 0,0 0 0,0-4 0,4 3 0,-3-3 0,3 0 0,-4 3 0,4 1 0,-3 1 0,2 3 0,-3-4 0,4 4 0,-3-3 0,-5 3 0,-6-8 0,-8 3 0,0-3 0,0 4 0,0 0 0,-13 2 0,10-2 0,-52 32 0,44-29 0,-44 28 0,52-38 0,-11 8 0,10-9 0,3 7 0,-3-3 0,4 4 0,0 0 0,-4-4 0,-20 26 0,14-20 0,-14 22 0,20-20 0,3-3 0,1-1 0,5-5 0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink27.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2021-08-25T14:02:25.390"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+      <inkml:brushProperty name="color" value="#E71224"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">2852 0 24575,'-13'0'0,"3"0"0,-36 0 0,28 0 0,-28 0 0,3 0 0,22 0 0,-35 0 0,40 0 0,-12 0 0,14 0 0,-3 0 0,-6 0 0,2 0 0,-34 0 0,-5 0 0,20 0 0,-19 0 0,2 0 0,27 0 0,-10 0 0,-14 0 0,-10 0 0,-4 0 0,-1 0 0,0 0 0,0 0 0,-14 0 0,9 0 0,24 0 0,-19 0 0,12 0 0,36 0 0,-35 0 0,40 0 0,-12 0 0,1 0 0,7 0 0,-4 0 0,11 0 0,4 0 0,-14 0 0,11 0 0,-10 0 0,-1 0 0,11 0 0,-15 0 0,13 4 0,0-3 0,1 7 0,-29-7 0,11 9 0,-18-4 0,25 4 0,11-1 0,4-4 0,-14 11 0,11-9 0,-10 10 0,-29 22 0,28-19 0,-29 20 0,25 6 0,14-28 0,-14 28 0,2-3 0,-6 12 0,2 9 0,5-19 0,11-9 0,7-23 0,1 9 0,5-9 0,-8 1 0,6 0 0,-6 3 0,2 7 0,4-8 0,-4 20 0,6-23 0,0 13 0,0-2 0,0-4 0,-4 8 0,3-1 0,-3-6 0,4 2 0,-9 23 0,7-24 0,-7 21 0,9 3 0,0-15 0,0 18 0,0 47 0,0-51 0,0 40 0,0 10 0,0-54 0,0 47 0,0-27 0,0-6 0,0-15 0,0 16 0,0 4 0,0 9 0,0-20 0,0 20 0,0-31 0,0-18 0,0 8 0,0 27 0,0-18 0,0 49 0,0-51 0,0 42 0,0-3 0,0 14 0,0-14 0,1-15 0,-2-2 0,-18 7 0,17-11 0,-1-2 0,-19-2 0,21-25 0,-3 2 0,4 20 0,-4-11 0,3 8 0,-3 3 0,4-29 0,-6 39 0,4-10 0,-3-11 0,-3 12 0,6 0 0,-6-22 0,4 22 0,3 1 0,-3-27 0,-2 35 0,4-40 0,-4 21 0,6-20 0,-9 38 0,7-33 0,-19 34 0,18-26 0,-9 0 0,12-2 0,-9 19 0,6-26 0,-6 35 0,5-40 0,3 8 0,-3 2 0,4-13 0,0 23 0,0-24 0,-4 15 0,3-13 0,-3 0 0,4-1 0,0-4 0,0 4 0,0-3 0,0 3 0,0-4 0,0 0 0,0 0 0,0 0 0,0-8 0,0-16 0,0 3 0,0-15 0,0-16 0,0 22 0,-9-55 0,-1 55 0,-6-22 0,-1 26 0,7 7 0,-3-3 0,5 0 0,-1 3 0,0-3 0,0 4 0,0 0 0,-4-4 0,7 3 0,-2-7 0,8 7 0,0-3 0,0-9 0,0 9 0,0-9 0,-12-1 0,9 11 0,-13-11 0,11 14 0,0-4 0,-3 3 0,3 1 0,-4 5 0,0 8 0,4 1 0,2 8 0,3 11 0,0-4 0,3 8 0,2-14 0,4 3 0,0-3 0,0 4 0,0-4 0,0 2 0,0-6 0,-4 7 0,-1-3 0,0 0 0,31 41 0,-22-36 0,27 45 0,-35-52 0,2 11 0,5-10 0,-10-3 0,6 3 0,-4-4 0,-3 4 0,21-1 0,-10-3 0,12-3 0,2-6 0,20 0 0,-11 0 0,41-19 0,-28-1 0,-2-2 0,14-11 0,-8 8 0,-9 5 0,-31 15 0,15-5 0,-17 9 0,3-7 0,-4 3 0,0-4 0,4 0 0,-3-4 0,3 3 0,0-7 0,10 5 0,-6-1 0,9-2 0,-12 5 0,14-5 0,-12 10 0,7-5 0,-14 5 0,-4 0 0,-1 1 0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink28.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2021-08-25T14:02:25.391"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+      <inkml:brushProperty name="color" value="#E71224"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">4048 1 24575,'-9'5'0,"-13"5"0,9-9 0,-23 5 0,10-6 0,-13 0 0,-20 0 0,28 0 0,-26 0 0,-1 0 0,17 0 0,-28 0 0,1 0 0,28 0 0,-36 0 0,6 0 0,31 0 0,-24 0 0,17 0 0,15 0 0,-15 0 0,20 0 0,2 0 0,8 0 0,-60 0 0,40 0 0,-33 0 0,-7 0 0,36 0 0,-29 0 0,20 18 0,2 2 0,2-10 0,-40 28 0,-10-25 0,35-10 0,11 6 0,-5 1 0,-8-10 0,6 1 0,1 11 0,-33-7 0,11 13 0,-21-11 0,32 5 0,-1-1 0,1-10 0,4 1 0,-12 13 0,-22 9 0,36-5 0,-23 12 0,22-19 0,4-1 0,2 10 0,-43-5 0,72-1 0,-28-2 0,-7 3 0,-12 29 0,16-25 0,2 0 0,1 19 0,44-30 0,-27 24 0,22-18 0,-42 41 0,38-37 0,-14 15 0,-11 21 0,13-3 0,-5 3 0,0 2 0,3 12 0,7-8 0,5-4 0,12-17 0,-2 36 0,11-60 0,0 60 0,0-40 0,0 33 0,0-12 0,0-32 0,0 32 0,0 31 0,0-33 0,0 43 0,0-39 0,0-24 0,0 42 0,0-3 0,0-5 0,0-8 0,0-4 0,0-18 0,0 28 0,0-39 0,0 2 0,0 0 0,0-3 0,0 1 0,11 2 0,-8 0 0,20 46 0,-20-36 0,9 29 0,-12 8 0,0-38 0,0 30 0,0 8 0,0-37 0,0 29 0,0 7 0,0-36 0,0 29 0,0 27 0,0-61 0,0 52 0,0-20 0,0-28 0,0 60 0,0-16 0,0-14 0,0 10 0,0 0 0,0-39 0,0 36 0,0-7 0,0-29 0,0 37 0,0-28 0,0-18 0,0 15 0,0-14 0,0 0 0,0 2 0,0-12 0,0 20 0,0-24 0,0 28 0,0-36 0,0 3 0,0-4 0,0 13 0,0-9 0,0 9 0,0-9 0,0-3 0,3 3 0,-2-4 0,3 4 0,2 11 0,-4-4 0,4 4 0,-6-12 0,0-3 0,0 4 0,0-3 0,0 7 0,0-3 0,0 0 0,0-1 0,0-4 0,0 4 0,0 1 0,0 0 0,0 3 0,0-7 0,0 3 0,0-4 0,0 4 0,0-3 0,0 36 0,0-29 0,0 25 0,0-33 0,0 4 0,4 1 0,1 0 0,0 13 0,-1-15 0,-4 3 0,0-16 0,-4-8 0,-1 0 0,-4-4 0,-4-1 0,3 0 0,1 1 0,5 4 0,0 0 0,-1 0 0,0 0 0,1 0 0,0 0 0,-1 0 0,-6-13 0,2 9 0,-2-9 0,2 13 0,0 0 0,0 0 0,0 0 0,0-4 0,0 3 0,0-7 0,0 7 0,4-3 0,-3 4 0,7 0 0,-3 0 0,4 0 0,-4 0 0,11 4 0,-5 5 0,11 5 0,-4 8 0,0 1 0,14 33 0,-2-12 0,4 11 0,0-10 0,-14-24 0,5 11 0,-7-14 0,-4 0 0,7 0 0,-6 0 0,15 13 0,-10-9 0,6 9 0,-4-13 0,-3 0 0,10 14 0,-13-19 0,5 9 0,-12-55 0,0 24 0,0-24 0,0 0 0,0 25 0,0-30 0,0 33 0,0 1 0,0-4 0,12-7 0,-9 4 0,36-28 0,-32 25 0,25-11 0,-31 21 0,3 8 0,-4 1 0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink29.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2021-08-25T14:02:25.392"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+      <inkml:brushProperty name="color" value="#E71224"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 199 24575,'13'0'0,"-3"0"0,3-4 0,9 3 0,-5-3 0,20 4 0,-17 0 0,76 0 0,-32 0 0,-1 0 0,11 0 0,-9 0 0,19 0-658,-10 0 1,13 0 0,-13 0 657,10 0 0,-20 0 0,9 0 0,-8 0-1095,28 0 1095,-12 0 0,0 0 0,13 0 0,-13 0 0,0 0 0,13 0 0,-4 0 0,1 0 0,8 0 0,-8 0 0,0 0 0,2 0 0,-12 0 0,0 0 0,13 0 0,-12 0 0,-2 0 0,-6 0 0,7 0 0,-5 0 0,-31 0 0,32 0 0,1 0 0,-34 0 0,25 0 0,0 0 0,-19 0 0,19 0 0,-1 0 0,-23 0 0,23 0 0,-1 0 0,-27 0 0,19-5 0,0-2 0,-19 5 0,18-4 0,-1 0 1856,-27 6-1856,29 0 0,-2 0 0,-31 0 0,69 0 1211,-73 0-1211,54 0 0,-55 0 0,55 0 0,-6 0 0,-11 0 0,8 0 0,-39 0 0,1 0 0,1 0 0,-2 0 0,-14 0 0,-1 0 0,-4 0 0,4 0 0,-3 0 0,3 0 0,-4 0 0,4 0 0,-3 0 0,3 0 0,-4 0 0,4 0 0,1-4 0,-5-1 0,-1-4 0,-8 0 0,-4 0 0,-1 0 0,-3 0 0,-5 0 0,3 4 0,-3-3 0,4 7 0,-39-7 0,-5-1 0,21 5 0,-19-2 0,-3-1 0,-9-5 0,33 9 0,-33-8 0,50 11 0,-10 0 0,11 0 0,-11-4 0,14-1 0,0-4 0,12 4 0,-1 1 0,11 4 0,0 0 0,1 4 0,54 11 0,10 1-2031,-33-4 2031,31 7 0,-11-4 0,-56-14 0,21 14 0,-16-8 0,17 6 0,-22-9 0,0-4 2031,0 4-2031,4-3 0,-3 7 0,3-7 0,-4 7 0,13 5 0,-9-6 0,9 4 0,-13-7 0,42 31 0,-40-22 0,30 25 0,-50-37 0,0 3 0,-4-4 0,3 0 0,-7 0 0,3 0 0,-53 0 0,37 0 0,-28 0 0,0 0 0,32 0 0,-40 0 0,56 0 0,-3 4 0,8 5 0,1 1 0,0 3 0,-1-4 0,-8 4 0,3 1 0,-3 0 0,4-1 0,1-8 0,-5-1 0,3-4 0,-7 0 0,7 0 0,-3 0 0,4 4 0,0 1 0,0 0 0,-4 3 0,3-7 0,-7 3 0,7 0 0,-3-3 0,4 7 0,4-7 0,1 3 0</inkml:trace>
+</inkml:ink>
+</file>
+
 <file path=xl/ink/ink3.xml><?xml version="1.0" encoding="utf-8"?>
 <inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
   <inkml:definitions>
@@ -1513,6 +3128,34 @@
     </inkml:brush>
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">3156 0 24575,'-9'4'0,"-41"31"0,26-22 0,-31 21 0,27-34 0,8 4 0,-8-3 0,14 3 0,1-4 0,1 0 0,2 0 0,-17 0 0,15 0 0,-15 0 0,4 0 0,6 0 0,-5 0 0,-21 0 0,26 0 0,-29 0 0,22 0 0,4 0 0,-4 0 0,8 0 0,2 0 0,0 0 0,1 0 0,4 0 0,-4 0 0,-11 0 0,-6 0 0,4 0 0,-10 0 0,24 0 0,-11 0 0,-19 0 0,25 0 0,-26 0 0,1 0 0,25 0 0,-29 0 0,22 0 0,4 0 0,-4 0 0,-41 0 0,42 0 0,-38 0 0,48 0 0,3 0 0,-7 0 0,3 0 0,-4 0 0,-10 0 0,12 0 0,-7 0 0,1 0 0,5 0 0,-6 0 0,6 0 0,-7 0 0,4 0 0,-8 0 0,1 0 0,11 0 0,-7 0 0,-19 0 0,24 0 0,-24 0 0,0 0 0,11 0 0,-14 0 0,-11 0 0,25 0 0,-28 0 0,33 0 0,-50 34 0,54-25 0,-53 25 0,62-34 0,-9 0 0,-20 0 0,24 0 0,-37 0 0,42 0 0,-23 0 0,20 0 0,-8 0 0,-22 18 0,29-13 0,-39 19 0,40-14 0,-8 2 0,11-3 0,4-5 0,0 0 0,-13 3 0,9-2 0,-25 21 0,-6 5 0,6-7 0,-30 34 0,31-20 0,6 1 0,9 18 0,-32 20 0,45-35 0,5-33 0,-9 13 0,7-9 0,-10 9 0,15-9 0,-7-3 0,1 17 0,-11 58 0,9-45 0,-3 20 0,2-5 0,7-38 0,-6 29 0,9-32 0,0 0 0,0-1 0,-4-4 0,3 4 0,-3-3 0,4 3 0,0 10 0,-4-7 0,-5 12 0,3-14 0,-2-1 0,8-4 0,0 0 0,0 13 0,-6 4 0,5 14 0,-5-14 0,6 0 0,0-2 0,0-4 0,0 4 0,0-7 0,0-3 0,0 0 0,0-2 0,0 11 0,0-11 0,0 11 0,0-14 0,-6 14 0,5-11 0,-5 10 0,6-9 0,0-3 0,0 56 0,0-44 0,0 40 0,0-49 0,0-3 0,0 3 0,0-4 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 4 0,0-3 0,0 3 0,0-4 0,0 13 0,0-9 0,0 9 0,0-9 0,0-3 0,0 36 0,0-28 0,0 24 0,0-33 0,-4 0 0,3 4 0,-3 50 0,4-37 0,0 36 0,0-50 0,0-2 0,0 3 0,0 49 0,0-40 0,0 44 0,0-56 0,0 3 0,0-4 0,0 4 0,-8 1 0,6 0 0,-6 3 0,4-7 0,3 3 0,1-4 0,1-8 0,3 2 0,-4-7 0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink30.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2021-08-25T14:02:25.393"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.2" units="cm"/>
+      <inkml:brushProperty name="height" value="0.2" units="cm"/>
+      <inkml:brushProperty name="color" value="#008C3A"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 1589 24575,'23'18'0,"14"26"0,-2 5 0,-13-13 0,6 12 0,0 6 0,1 35 0,-18-44 0,4 1 0,2 4 0,14 39 0,-7-27 0,-7-11 0,0-2 0,2-1 0,-11-22 0,-3-4 0,-5-9 0,4-3 0,-3 3 0,11 0 0,2 11 0,-3-8 0,12 20 0,-16-23 0,43 5 0,-28-14 0,34-4 0,-35-4 0,43-29 0,12-10 0,-30 21 0,2-2-695,22-13 0,10-8 1,1 5 694,-3 12 0,0 3 0,2-1-1093,2-6 1,1-1 0,2 2 984,5 2 0,3 2 1,4-2 107,-22 6 0,5-1 0,2 0 0,-2 0 0,-4 1-820,0 0 1,-5 1 0,1 0 0,4 0 753,15-4 1,3 0-1,4 0 1,2-2 65,-7 1 0,4 0 0,2-2 0,-5 1 0,-6 0-791,-12 1 0,-7 1 1,0 0-1,7-2 791,-3 3 0,5 0 0,4-1 0,1-1 0,-1-1 0,-4-2 0,6-7 0,0-2 0,-3-2 0,-2 2 0,-2 3 0,-1 1 0,-4 3 0,0 1 0,3-2 0,-2-1 0,2 0 0,2-2 0,-1 1 0,-1 3 0,11-3 0,0 2 0,-3 0 0,-4 0-690,1-6 1,-6 1 0,4-2 689,-10 9 0,3 0 0,1-1 0,-4-4 0,0-6 0,-1-5 0,-3 0 0,-7 7-155,6-2 0,-3 3 155,2-5 0,4-3 0,-5 8 359,-7 13 0,-10 8 1,-12 0-1,25-4 1</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -1984,7 +3627,7 @@
   <dimension ref="B2:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="21" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1999,13 +3642,13 @@
     </row>
     <row r="3" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>9</v>
-      </c>
       <c r="D3" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>1</v>
@@ -2016,13 +3659,13 @@
         <v>4</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2030,61 +3673,61 @@
         <v>5</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>6</v>
+        <v>62</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="D9" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>9</v>
-      </c>
       <c r="D14" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>1</v>
@@ -2092,56 +3735,56 @@
     </row>
     <row r="15" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>18</v>
+        <v>60</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>5</v>
+        <v>59</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
-        <v>21</v>
+        <v>61</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -2156,8 +3799,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F0C55FB-E51F-DF4E-8CE7-0FAC2332E562}">
   <dimension ref="B2:S47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="R27" sqref="R27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2171,10 +3814,10 @@
   <sheetData>
     <row r="2" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" t="s">
         <v>24</v>
-      </c>
-      <c r="E2" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.2">
@@ -2184,7 +3827,7 @@
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.2">
       <c r="D4" s="7" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E4" s="8"/>
       <c r="F4" s="9"/>
@@ -2196,7 +3839,7 @@
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.2">
       <c r="D6" s="7" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E6" s="8"/>
       <c r="F6" s="9"/>
@@ -2228,16 +3871,16 @@
     </row>
     <row r="14" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" t="s">
+        <v>26</v>
+      </c>
+      <c r="F14" t="s">
+        <v>27</v>
+      </c>
+      <c r="G14" t="s">
         <v>28</v>
-      </c>
-      <c r="C14" t="s">
-        <v>29</v>
-      </c>
-      <c r="F14" t="s">
-        <v>30</v>
-      </c>
-      <c r="G14" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.2">
@@ -2314,28 +3957,28 @@
     </row>
     <row r="26" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D26" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E26" t="s">
+        <v>51</v>
+      </c>
+      <c r="I26" t="s">
         <v>54</v>
       </c>
-      <c r="I26" t="s">
-        <v>57</v>
-      </c>
       <c r="J26" t="s">
+        <v>63</v>
+      </c>
+      <c r="M26" t="s">
         <v>58</v>
-      </c>
-      <c r="M26" t="s">
-        <v>63</v>
       </c>
       <c r="N26" t="s">
         <v>64</v>
       </c>
       <c r="Q26" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="R26" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="27" spans="2:19" x14ac:dyDescent="0.2">
@@ -2354,7 +3997,7 @@
     </row>
     <row r="28" spans="2:19" x14ac:dyDescent="0.2">
       <c r="D28" s="15" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E28" s="8"/>
       <c r="F28" s="9"/>
@@ -2375,7 +4018,7 @@
       <c r="E29" s="8"/>
       <c r="F29" s="9"/>
       <c r="I29" s="7" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="J29" s="8"/>
       <c r="K29" s="9"/>
@@ -2388,12 +4031,12 @@
     </row>
     <row r="30" spans="2:19" x14ac:dyDescent="0.2">
       <c r="D30" s="14" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E30" s="8"/>
       <c r="F30" s="9"/>
       <c r="I30" s="7" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="J30" s="8"/>
       <c r="K30" s="9"/>
@@ -2409,7 +4052,7 @@
       <c r="E31" s="8"/>
       <c r="F31" s="9"/>
       <c r="I31" s="7" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="J31" s="8"/>
       <c r="K31" s="9"/>
@@ -2422,7 +4065,7 @@
     </row>
     <row r="32" spans="2:19" x14ac:dyDescent="0.2">
       <c r="D32" s="15" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E32" s="8"/>
       <c r="F32" s="9"/>
@@ -2452,7 +4095,7 @@
     </row>
     <row r="34" spans="2:19" x14ac:dyDescent="0.2">
       <c r="D34" s="15" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E34" s="8"/>
       <c r="F34" s="9"/>
@@ -2482,22 +4125,22 @@
     </row>
     <row r="38" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C38" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F38" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G38" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="K38" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="L38" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="39" spans="2:19" x14ac:dyDescent="0.2">
@@ -2514,14 +4157,14 @@
     </row>
     <row r="40" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B40" s="7" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D40" s="9"/>
       <c r="F40" s="7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G40" s="8"/>
       <c r="H40" s="8"/>
@@ -2530,33 +4173,33 @@
         <v>2</v>
       </c>
       <c r="L40" s="8" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="M40" s="9"/>
     </row>
     <row r="41" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B41" s="7" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D41" s="9"/>
       <c r="F41" s="7"/>
       <c r="G41" s="8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="H41" s="8" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="I41" s="9" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="K41" s="7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="L41" s="8" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="M41" s="9"/>
     </row>
@@ -2572,7 +4215,7 @@
         <v>3</v>
       </c>
       <c r="L42" s="13" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="M42" s="9"/>
     </row>
@@ -2617,12 +4260,12 @@
       <c r="C46" s="8"/>
       <c r="D46" s="9"/>
       <c r="F46" s="7" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G46" s="8"/>
       <c r="H46" s="8"/>
       <c r="I46" s="9" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="K46" s="7"/>
       <c r="L46" s="8"/>
@@ -2644,4 +4287,498 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D45E1F2-172E-714D-8274-891E81A9922E}">
+  <dimension ref="B2:S47"/>
+  <sheetViews>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="S38" sqref="S38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="12.1640625" customWidth="1"/>
+    <col min="7" max="7" width="11.83203125" customWidth="1"/>
+    <col min="9" max="9" width="11.5" customWidth="1"/>
+    <col min="11" max="11" width="13.1640625" customWidth="1"/>
+    <col min="13" max="13" width="12.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="D3" s="4"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="6"/>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="D4" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="8"/>
+      <c r="F4" s="9"/>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="D5" s="7"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="9"/>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="D6" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="8"/>
+      <c r="F6" s="9"/>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="D7" s="7"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="9"/>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="D8" s="7"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="9"/>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="D9" s="7"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="9"/>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="D10" s="7"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="9"/>
+    </row>
+    <row r="11" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D11" s="10"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="12"/>
+    </row>
+    <row r="14" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" t="s">
+        <v>26</v>
+      </c>
+      <c r="F14" t="s">
+        <v>27</v>
+      </c>
+      <c r="G14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B15" s="4"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="6"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="6"/>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B16" s="7"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="9"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="9"/>
+    </row>
+    <row r="17" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B17" s="7"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="9"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="9"/>
+    </row>
+    <row r="18" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B18" s="7"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="9"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="9"/>
+    </row>
+    <row r="19" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B19" s="7"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="9"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="9"/>
+    </row>
+    <row r="20" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B20" s="7"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="9"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="9"/>
+    </row>
+    <row r="21" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B21" s="7"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="9"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="9"/>
+    </row>
+    <row r="22" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B22" s="7"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="9"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="9"/>
+    </row>
+    <row r="23" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="10"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="12"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="12"/>
+    </row>
+    <row r="26" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D26" t="s">
+        <v>50</v>
+      </c>
+      <c r="E26" t="s">
+        <v>51</v>
+      </c>
+      <c r="I26" t="s">
+        <v>54</v>
+      </c>
+      <c r="J26" t="s">
+        <v>63</v>
+      </c>
+      <c r="M26" t="s">
+        <v>58</v>
+      </c>
+      <c r="N26" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>57</v>
+      </c>
+      <c r="R26" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="27" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="D27" s="4"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="6"/>
+      <c r="I27" s="4"/>
+      <c r="J27" s="5"/>
+      <c r="K27" s="6"/>
+      <c r="M27" s="4"/>
+      <c r="N27" s="5"/>
+      <c r="O27" s="6"/>
+      <c r="Q27" s="4"/>
+      <c r="R27" s="5"/>
+      <c r="S27" s="6"/>
+    </row>
+    <row r="28" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="D28" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="E28" s="8"/>
+      <c r="F28" s="9"/>
+      <c r="I28" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="J28" s="8"/>
+      <c r="K28" s="9"/>
+      <c r="M28" s="7"/>
+      <c r="N28" s="8"/>
+      <c r="O28" s="9"/>
+      <c r="Q28" s="7"/>
+      <c r="R28" s="8"/>
+      <c r="S28" s="9"/>
+    </row>
+    <row r="29" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="D29" s="7"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="9"/>
+      <c r="I29" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="J29" s="8"/>
+      <c r="K29" s="9"/>
+      <c r="M29" s="7"/>
+      <c r="N29" s="8"/>
+      <c r="O29" s="9"/>
+      <c r="Q29" s="7"/>
+      <c r="R29" s="8"/>
+      <c r="S29" s="9"/>
+    </row>
+    <row r="30" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="D30" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E30" s="8"/>
+      <c r="F30" s="9"/>
+      <c r="I30" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="J30" s="8"/>
+      <c r="K30" s="9"/>
+      <c r="M30" s="7"/>
+      <c r="N30" s="8"/>
+      <c r="O30" s="9"/>
+      <c r="Q30" s="7"/>
+      <c r="R30" s="8"/>
+      <c r="S30" s="9"/>
+    </row>
+    <row r="31" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="D31" s="7"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="9"/>
+      <c r="I31" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="J31" s="8"/>
+      <c r="K31" s="9"/>
+      <c r="M31" s="7"/>
+      <c r="N31" s="8"/>
+      <c r="O31" s="9"/>
+      <c r="Q31" s="7"/>
+      <c r="R31" s="8"/>
+      <c r="S31" s="9"/>
+    </row>
+    <row r="32" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="D32" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="E32" s="8"/>
+      <c r="F32" s="9"/>
+      <c r="I32" s="7"/>
+      <c r="J32" s="8"/>
+      <c r="K32" s="9"/>
+      <c r="M32" s="7"/>
+      <c r="N32" s="8"/>
+      <c r="O32" s="9"/>
+      <c r="Q32" s="7"/>
+      <c r="R32" s="8"/>
+      <c r="S32" s="9"/>
+    </row>
+    <row r="33" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="D33" s="7"/>
+      <c r="E33" s="8"/>
+      <c r="F33" s="9"/>
+      <c r="I33" s="7"/>
+      <c r="J33" s="8"/>
+      <c r="K33" s="9"/>
+      <c r="M33" s="7"/>
+      <c r="N33" s="8"/>
+      <c r="O33" s="9"/>
+      <c r="Q33" s="7"/>
+      <c r="R33" s="8"/>
+      <c r="S33" s="9"/>
+    </row>
+    <row r="34" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="D34" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="E34" s="8"/>
+      <c r="F34" s="9"/>
+      <c r="I34" s="7"/>
+      <c r="J34" s="8"/>
+      <c r="K34" s="9"/>
+      <c r="M34" s="7"/>
+      <c r="N34" s="8"/>
+      <c r="O34" s="9"/>
+      <c r="Q34" s="7"/>
+      <c r="R34" s="8"/>
+      <c r="S34" s="9"/>
+    </row>
+    <row r="35" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D35" s="10"/>
+      <c r="E35" s="11"/>
+      <c r="F35" s="12"/>
+      <c r="I35" s="10"/>
+      <c r="J35" s="11"/>
+      <c r="K35" s="12"/>
+      <c r="M35" s="10"/>
+      <c r="N35" s="11"/>
+      <c r="O35" s="12"/>
+      <c r="Q35" s="10"/>
+      <c r="R35" s="11"/>
+      <c r="S35" s="12"/>
+    </row>
+    <row r="38" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>37</v>
+      </c>
+      <c r="C38" t="s">
+        <v>38</v>
+      </c>
+      <c r="F38" t="s">
+        <v>29</v>
+      </c>
+      <c r="G38" t="s">
+        <v>30</v>
+      </c>
+      <c r="K38" t="s">
+        <v>39</v>
+      </c>
+      <c r="L38" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="39" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B39" s="4"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="6"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="5"/>
+      <c r="H39" s="5"/>
+      <c r="I39" s="6"/>
+      <c r="K39" s="4"/>
+      <c r="L39" s="5"/>
+      <c r="M39" s="6"/>
+    </row>
+    <row r="40" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B40" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D40" s="9"/>
+      <c r="F40" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G40" s="8"/>
+      <c r="H40" s="8"/>
+      <c r="I40" s="9"/>
+      <c r="K40" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="L40" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="M40" s="9"/>
+    </row>
+    <row r="41" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B41" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D41" s="9"/>
+      <c r="F41" s="7"/>
+      <c r="G41" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H41" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="I41" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="K41" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="L41" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="M41" s="9"/>
+    </row>
+    <row r="42" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B42" s="7"/>
+      <c r="C42" s="8"/>
+      <c r="D42" s="9"/>
+      <c r="F42" s="7"/>
+      <c r="G42" s="8"/>
+      <c r="H42" s="8"/>
+      <c r="I42" s="9"/>
+      <c r="K42" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="L42" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="M42" s="9"/>
+    </row>
+    <row r="43" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B43" s="7"/>
+      <c r="C43" s="8"/>
+      <c r="D43" s="9"/>
+      <c r="F43" s="7"/>
+      <c r="G43" s="8"/>
+      <c r="H43" s="8"/>
+      <c r="I43" s="9"/>
+      <c r="K43" s="7"/>
+      <c r="L43" s="8"/>
+      <c r="M43" s="9"/>
+    </row>
+    <row r="44" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B44" s="7"/>
+      <c r="C44" s="8"/>
+      <c r="D44" s="9"/>
+      <c r="F44" s="7"/>
+      <c r="G44" s="8"/>
+      <c r="H44" s="8"/>
+      <c r="I44" s="9"/>
+      <c r="K44" s="7"/>
+      <c r="L44" s="8"/>
+      <c r="M44" s="9"/>
+    </row>
+    <row r="45" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B45" s="7"/>
+      <c r="C45" s="8"/>
+      <c r="D45" s="9"/>
+      <c r="F45" s="7"/>
+      <c r="G45" s="8"/>
+      <c r="H45" s="8"/>
+      <c r="I45" s="9"/>
+      <c r="K45" s="7"/>
+      <c r="L45" s="8"/>
+      <c r="M45" s="9"/>
+    </row>
+    <row r="46" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B46" s="7"/>
+      <c r="C46" s="8"/>
+      <c r="D46" s="9"/>
+      <c r="F46" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G46" s="8"/>
+      <c r="H46" s="8"/>
+      <c r="I46" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="K46" s="7"/>
+      <c r="L46" s="8"/>
+      <c r="M46" s="9"/>
+    </row>
+    <row r="47" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="10"/>
+      <c r="C47" s="11"/>
+      <c r="D47" s="12"/>
+      <c r="F47" s="10"/>
+      <c r="G47" s="11"/>
+      <c r="H47" s="11"/>
+      <c r="I47" s="12"/>
+      <c r="K47" s="10"/>
+      <c r="L47" s="11"/>
+      <c r="M47" s="12"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>